<commit_message>
Add Pryzm cATOM exchange rate integration with real live data
- Add Pryzm service for live exchange rate fetching
- Add Pryzm hook for UI integration with APR calculations
- Add snapshot script for Pryzm exchange rate data
- Update package.json with Pryzm snapshot scripts
- Fix APR calculation to require minimum time periods
- Remove Alliance APR implementation files
</commit_message>
<xml_diff>
--- a/src/pages/tabs/data/Daily APR.xlsx
+++ b/src/pages/tabs/data/Daily APR.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -444,12 +444,23 @@
         <v>2025-08-29T14:45</v>
       </c>
       <c r="C4">
-        <v>1.6687217860323946</v>
+        <v>1.6694299880323946</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2025-08-31T13:39</v>
+      </c>
+      <c r="C5">
+        <v>1.6703984340747713</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: Update branding to UseAtom and improve liquid staking
- Change site title from cosmos-flux-lab to UseAtom
- Add new SVG atom favicon with ICO fallback
- Remove Milky Way from liquid staking protocols
- Set Pryzm protocol fee to 10% of rewards
- Update Open Graph title for social sharing
</commit_message>
<xml_diff>
--- a/src/pages/tabs/data/Daily APR.xlsx
+++ b/src/pages/tabs/data/Daily APR.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -458,9 +458,20 @@
         <v>1.6703984340747713</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2025-09-01T22:16</v>
+      </c>
+      <c r="C6">
+        <v>1.6714039663513292</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix Buffer.alloc error in LedgerWalletAdapter and update dependencies
</commit_message>
<xml_diff>
--- a/src/pages/tabs/data/Daily APR.xlsx
+++ b/src/pages/tabs/data/Daily APR.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -469,9 +469,20 @@
         <v>1.6714039663513292</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2025-09-02T09:30</v>
+      </c>
+      <c r="C7">
+        <v>1.6718133009139704</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Remove Inter Protocol from Lending, add App.calculated.fi to Others, update snapshot data
</commit_message>
<xml_diff>
--- a/src/pages/tabs/data/Daily APR.xlsx
+++ b/src/pages/tabs/data/Daily APR.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -480,9 +480,20 @@
         <v>1.6718133009139704</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2025-09-11T09:31</v>
+      </c>
+      <c r="C8">
+        <v>1.6792199976262983</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Optimize entire website for mobile without removing features
- Make all tables horizontally scrollable on mobile with min-widths
- Improve ProtocolCard responsiveness (metrics grid, action button wrapping)
- Enhance Header layout for mobile (tighter spacing, responsive search, hidden 'Swap' text)
- Make SwapPanel dialog and widget responsive to viewport height
- Add mobile utilities (no-scrollbar, safe-area helpers)
- Update viewport meta for notched devices
- Implement chain-aware ATOM balance check with swap popup
- Integrate balance check into liquidity pool links
- Update SwapWidget to target destination chain for ATOM swaps
</commit_message>
<xml_diff>
--- a/src/pages/tabs/data/Daily APR.xlsx
+++ b/src/pages/tabs/data/Daily APR.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -491,9 +491,20 @@
         <v>1.6792199976262983</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2025-09-20T11:39</v>
+      </c>
+      <c r="C9">
+        <v>1.6866366606922056</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update data files from latest scraping and snapshot runs
</commit_message>
<xml_diff>
--- a/src/pages/tabs/data/Daily APR.xlsx
+++ b/src/pages/tabs/data/Daily APR.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -502,9 +502,20 @@
         <v>1.6866366606922056</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2025-10-11T20:33</v>
+      </c>
+      <c r="C10">
+        <v>1.7042856802003863</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>